<commit_message>
Added cluster data analysis
</commit_message>
<xml_diff>
--- a/Data Results_test_07.xlsx
+++ b/Data Results_test_07.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Renato\CLionProjects\cp2020-2021_g26_45616_52360_52393\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49ED99E0-1351-44DD-AB02-57B4527C1C36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DDAB57F-982F-49E3-BCBC-DCC23D06731C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="2" xr2:uid="{FE04AF36-4D43-4F52-8DE8-9BA373B3A9EA}"/>
+    <workbookView xWindow="-8328" yWindow="3192" windowWidth="17280" windowHeight="9072" xr2:uid="{FE04AF36-4D43-4F52-8DE8-9BA373B3A9EA}"/>
   </bookViews>
   <sheets>
     <sheet name="1 File" sheetId="2" r:id="rId1"/>
@@ -793,36 +793,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -830,12 +800,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
@@ -870,6 +834,42 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5659,8 +5659,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CECB3340-A37B-4887-BE35-D30BA3446E8B}">
   <dimension ref="A1:C44"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="E40" sqref="E40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5671,11 +5671,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="66" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="51"/>
-      <c r="C1" s="52"/>
+      <c r="B1" s="67"/>
+      <c r="C1" s="68"/>
     </row>
     <row r="2" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="26" t="s">
@@ -6145,11 +6145,11 @@
       <c r="A44" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="B44" s="53">
+      <c r="B44" s="69">
         <f>B43/C43</f>
         <v>6.434752483128654</v>
       </c>
-      <c r="C44" s="54"/>
+      <c r="C44" s="70"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -6166,7 +6166,7 @@
   <dimension ref="A1:L44"/>
   <sheetViews>
     <sheetView zoomScale="72" workbookViewId="0">
-      <selection activeCell="I38" sqref="I38"/>
+      <selection activeCell="C3" sqref="C3:C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6177,11 +6177,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="66" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="51"/>
-      <c r="C1" s="52"/>
+      <c r="B1" s="67"/>
+      <c r="C1" s="68"/>
     </row>
     <row r="2" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="26" t="s">
@@ -7160,11 +7160,11 @@
       <c r="A44" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="B44" s="53">
+      <c r="B44" s="69">
         <f>B43/C43</f>
         <v>6.5619875903389859</v>
       </c>
-      <c r="C44" s="54"/>
+      <c r="C44" s="70"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -7180,8 +7180,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B54125CA-857F-4D0F-97EC-C1C08DAC287C}">
   <dimension ref="A1:O44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B6" zoomScale="116" workbookViewId="0">
-      <selection activeCell="D44" sqref="D44"/>
+    <sheetView topLeftCell="F1" zoomScale="70" workbookViewId="0">
+      <selection activeCell="O4" sqref="O4:O13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7196,13 +7196,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="57" t="s">
+      <c r="A1" s="73" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="58"/>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
-      <c r="E1" s="59"/>
+      <c r="B1" s="74"/>
+      <c r="C1" s="74"/>
+      <c r="D1" s="74"/>
+      <c r="E1" s="75"/>
     </row>
     <row r="2" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="43" t="s">
@@ -7243,13 +7243,13 @@
       <c r="L3" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="M3" s="62" t="s">
+      <c r="M3" s="52" t="s">
         <v>2</v>
       </c>
-      <c r="N3" s="69" t="s">
+      <c r="N3" s="57" t="s">
         <v>10</v>
       </c>
-      <c r="O3" s="69" t="s">
+      <c r="O3" s="57" t="s">
         <v>11</v>
       </c>
     </row>
@@ -7269,7 +7269,7 @@
       <c r="E4" s="18">
         <v>16.599968000000001</v>
       </c>
-      <c r="K4" s="60">
+      <c r="K4" s="50">
         <v>1</v>
       </c>
       <c r="L4" s="2">
@@ -7301,19 +7301,19 @@
       <c r="E5" s="18">
         <v>16.630718999999999</v>
       </c>
-      <c r="K5" s="71">
+      <c r="K5" s="59">
         <v>2</v>
       </c>
-      <c r="L5" s="72">
+      <c r="L5" s="60">
         <v>104.648702</v>
       </c>
-      <c r="M5" s="75">
+      <c r="M5" s="63">
         <v>15.929888999999999</v>
       </c>
-      <c r="N5" s="73">
+      <c r="N5" s="61">
         <v>16.585601</v>
       </c>
-      <c r="O5" s="73">
+      <c r="O5" s="61">
         <v>16.599968000000001</v>
       </c>
     </row>
@@ -7333,7 +7333,7 @@
       <c r="E6" s="18">
         <v>16.631056999999998</v>
       </c>
-      <c r="K6" s="61">
+      <c r="K6" s="51">
         <v>3</v>
       </c>
       <c r="L6" s="1">
@@ -7365,19 +7365,19 @@
       <c r="E7" s="18">
         <v>16.639078999999999</v>
       </c>
-      <c r="K7" s="71">
+      <c r="K7" s="59">
         <v>4</v>
       </c>
-      <c r="L7" s="72">
+      <c r="L7" s="60">
         <v>105.218778</v>
       </c>
-      <c r="M7" s="75">
+      <c r="M7" s="63">
         <v>16.030422000000002</v>
       </c>
-      <c r="N7" s="73">
+      <c r="N7" s="61">
         <v>16.640356000000001</v>
       </c>
-      <c r="O7" s="73">
+      <c r="O7" s="61">
         <v>16.631056999999998</v>
       </c>
     </row>
@@ -7397,7 +7397,7 @@
       <c r="E8" s="18">
         <v>16.647072999999999</v>
       </c>
-      <c r="K8" s="61">
+      <c r="K8" s="51">
         <v>5</v>
       </c>
       <c r="L8" s="1">
@@ -7417,7 +7417,7 @@
       <c r="A9" s="28">
         <v>7</v>
       </c>
-      <c r="B9" s="77">
+      <c r="B9" s="65">
         <v>104.734859</v>
       </c>
       <c r="C9" s="18">
@@ -7429,19 +7429,19 @@
       <c r="E9" s="18">
         <v>16.652567000000001</v>
       </c>
-      <c r="K9" s="71">
+      <c r="K9" s="59">
         <v>6</v>
       </c>
-      <c r="L9" s="72">
+      <c r="L9" s="60">
         <v>105.310193</v>
       </c>
-      <c r="M9" s="75">
+      <c r="M9" s="63">
         <v>16.198853</v>
       </c>
-      <c r="N9" s="73">
+      <c r="N9" s="61">
         <v>16.653676999999998</v>
       </c>
-      <c r="O9" s="73">
+      <c r="O9" s="61">
         <v>16.647072999999999</v>
       </c>
     </row>
@@ -7449,7 +7449,7 @@
       <c r="A10" s="28">
         <v>8</v>
       </c>
-      <c r="B10" s="77">
+      <c r="B10" s="65">
         <v>104.96854500000001</v>
       </c>
       <c r="C10" s="18">
@@ -7461,7 +7461,7 @@
       <c r="E10" s="18">
         <v>16.660705</v>
       </c>
-      <c r="K10" s="61">
+      <c r="K10" s="51">
         <v>7</v>
       </c>
       <c r="L10" s="37">
@@ -7481,7 +7481,7 @@
       <c r="A11" s="28">
         <v>9</v>
       </c>
-      <c r="B11" s="77">
+      <c r="B11" s="65">
         <v>105.288856</v>
       </c>
       <c r="C11" s="18">
@@ -7493,19 +7493,19 @@
       <c r="E11" s="18">
         <v>16.680819</v>
       </c>
-      <c r="K11" s="71">
+      <c r="K11" s="59">
         <v>8</v>
       </c>
-      <c r="L11" s="76">
+      <c r="L11" s="64">
         <v>104.96854500000001</v>
       </c>
-      <c r="M11" s="75">
+      <c r="M11" s="63">
         <v>16.286193999999998</v>
       </c>
-      <c r="N11" s="73">
+      <c r="N11" s="61">
         <v>16.673428000000001</v>
       </c>
-      <c r="O11" s="73">
+      <c r="O11" s="61">
         <v>16.660705</v>
       </c>
     </row>
@@ -7513,7 +7513,7 @@
       <c r="A12" s="28">
         <v>10</v>
       </c>
-      <c r="B12" s="77">
+      <c r="B12" s="65">
         <v>105.34578999999999</v>
       </c>
       <c r="C12" s="18">
@@ -7525,7 +7525,7 @@
       <c r="E12" s="18">
         <v>16.682485</v>
       </c>
-      <c r="K12" s="61">
+      <c r="K12" s="51">
         <v>9</v>
       </c>
       <c r="L12" s="37">
@@ -7545,7 +7545,7 @@
       <c r="A13" s="28">
         <v>11</v>
       </c>
-      <c r="B13" s="77">
+      <c r="B13" s="65">
         <v>105.387294</v>
       </c>
       <c r="C13" s="18">
@@ -7557,19 +7557,19 @@
       <c r="E13" s="18">
         <v>16.703575000000001</v>
       </c>
-      <c r="K13" s="71">
+      <c r="K13" s="59">
         <v>10</v>
       </c>
-      <c r="L13" s="76">
+      <c r="L13" s="64">
         <v>105.34578999999999</v>
       </c>
-      <c r="M13" s="75">
+      <c r="M13" s="63">
         <v>16.579771000000001</v>
       </c>
-      <c r="N13" s="73">
+      <c r="N13" s="61">
         <v>16.679659000000001</v>
       </c>
-      <c r="O13" s="73">
+      <c r="O13" s="61">
         <v>16.682485</v>
       </c>
     </row>
@@ -7577,7 +7577,7 @@
       <c r="A14" s="28">
         <v>12</v>
       </c>
-      <c r="B14" s="77">
+      <c r="B14" s="65">
         <v>105.388964</v>
       </c>
       <c r="C14" s="18">
@@ -7589,7 +7589,7 @@
       <c r="E14" s="18">
         <v>16.726603000000001</v>
       </c>
-      <c r="K14" s="61">
+      <c r="K14" s="51">
         <v>11</v>
       </c>
       <c r="L14" s="37">
@@ -7609,7 +7609,7 @@
       <c r="A15" s="28">
         <v>13</v>
       </c>
-      <c r="B15" s="77">
+      <c r="B15" s="65">
         <v>105.527028</v>
       </c>
       <c r="C15" s="18">
@@ -7621,19 +7621,19 @@
       <c r="E15" s="18">
         <v>16.740797000000001</v>
       </c>
-      <c r="K15" s="71">
+      <c r="K15" s="59">
         <v>12</v>
       </c>
-      <c r="L15" s="76">
+      <c r="L15" s="64">
         <v>105.388964</v>
       </c>
-      <c r="M15" s="75">
+      <c r="M15" s="63">
         <v>16.754182</v>
       </c>
-      <c r="N15" s="73">
+      <c r="N15" s="61">
         <v>16.688614000000001</v>
       </c>
-      <c r="O15" s="73">
+      <c r="O15" s="61">
         <v>16.726603000000001</v>
       </c>
     </row>
@@ -7641,7 +7641,7 @@
       <c r="A16" s="28">
         <v>14</v>
       </c>
-      <c r="B16" s="77">
+      <c r="B16" s="65">
         <v>106.804677</v>
       </c>
       <c r="C16" s="18">
@@ -7653,7 +7653,7 @@
       <c r="E16" s="18">
         <v>16.743559000000001</v>
       </c>
-      <c r="K16" s="61">
+      <c r="K16" s="51">
         <v>13</v>
       </c>
       <c r="L16" s="37">
@@ -7673,7 +7673,7 @@
       <c r="A17" s="28">
         <v>15</v>
       </c>
-      <c r="B17" s="77">
+      <c r="B17" s="65">
         <v>111.795377</v>
       </c>
       <c r="C17" s="18">
@@ -7685,19 +7685,19 @@
       <c r="E17" s="18">
         <v>16.747917999999999</v>
       </c>
-      <c r="K17" s="71">
+      <c r="K17" s="59">
         <v>14</v>
       </c>
-      <c r="L17" s="76">
+      <c r="L17" s="64">
         <v>106.804677</v>
       </c>
-      <c r="M17" s="75">
+      <c r="M17" s="63">
         <v>16.873629000000001</v>
       </c>
-      <c r="N17" s="73">
+      <c r="N17" s="61">
         <v>16.710066999999999</v>
       </c>
-      <c r="O17" s="73">
+      <c r="O17" s="61">
         <v>16.743559000000001</v>
       </c>
     </row>
@@ -7705,7 +7705,7 @@
       <c r="A18" s="28">
         <v>16</v>
       </c>
-      <c r="B18" s="77">
+      <c r="B18" s="65">
         <v>119.16439</v>
       </c>
       <c r="C18" s="18">
@@ -7717,7 +7717,7 @@
       <c r="E18" s="18">
         <v>16.752168999999999</v>
       </c>
-      <c r="K18" s="61">
+      <c r="K18" s="51">
         <v>15</v>
       </c>
       <c r="L18" s="36">
@@ -7750,19 +7750,19 @@
       <c r="K19" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="L19" s="66">
+      <c r="L19" s="54">
         <f>AVERAGE(L4:L18)</f>
         <v>105.67712059999999</v>
       </c>
-      <c r="M19" s="74">
+      <c r="M19" s="62">
         <f>AVERAGE(M4:M18)</f>
         <v>16.372470266666667</v>
       </c>
-      <c r="N19" s="68">
+      <c r="N19" s="56">
         <f t="shared" ref="N19:O19" si="0">AVERAGE(N4:N18)</f>
         <v>16.647312200000002</v>
       </c>
-      <c r="O19" s="65">
+      <c r="O19" s="53">
         <f t="shared" si="0"/>
         <v>16.7253826</v>
       </c>
@@ -7781,19 +7781,19 @@
       <c r="E20" s="18">
         <v>16.768401000000001</v>
       </c>
-      <c r="K20" s="63" t="s">
+      <c r="K20" s="76" t="s">
         <v>7</v>
       </c>
-      <c r="L20" s="64"/>
-      <c r="M20" s="67">
+      <c r="L20" s="77"/>
+      <c r="M20" s="55">
         <f>L19/M19</f>
         <v>6.4545617661100323</v>
       </c>
-      <c r="N20" s="70">
+      <c r="N20" s="58">
         <f>L19/N19</f>
         <v>6.347998964060996</v>
       </c>
-      <c r="O20" s="70">
+      <c r="O20" s="58">
         <f>L19/O19</f>
         <v>6.3183679038828089</v>
       </c>
@@ -8153,11 +8153,11 @@
       <c r="A44" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="B44" s="55">
+      <c r="B44" s="71">
         <f>B43/C43</f>
         <v>6.2689848380217903</v>
       </c>
-      <c r="C44" s="56"/>
+      <c r="C44" s="72"/>
       <c r="D44" s="14">
         <f>B43/D43</f>
         <v>6.3314137179928762</v>

</xml_diff>